<commit_message>
hopefully cleaning up stuff
</commit_message>
<xml_diff>
--- a/koboforms/section1.xlsx
+++ b/koboforms/section1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deo/generateKobo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deo/whatsthepointgameinteractive/koboforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFD120D-306F-B942-9BF8-307C0D45FEB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE552F1-55C6-CB4B-A6B5-8412E1E65C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32500" yWindow="-22380" windowWidth="28040" windowHeight="17440" xr2:uid="{05574417-E28B-7A44-8D51-6FA488FA6DA5}"/>
+    <workbookView xWindow="-32500" yWindow="-22380" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{05574417-E28B-7A44-8D51-6FA488FA6DA5}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -102,10 +102,10 @@
     <t>Don’t Invest</t>
   </si>
   <si>
-    <t>WhatsThePointGameInteractive_Section1</t>
-  </si>
-  <si>
     <t>Your email</t>
+  </si>
+  <si>
+    <t>Take a chance?</t>
   </si>
 </sst>
 </file>
@@ -468,7 +468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{994C7F9E-9867-6243-AAB9-77628DC2993D}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -499,7 +499,7 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -576,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8DF2FC2-2B0D-0B42-899E-2C094C966549}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -595,7 +595,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>

</xml_diff>